<commit_message>
10- resolvendo erro na atulizacao na base de dados
</commit_message>
<xml_diff>
--- a/003-importacaoETratamentoDeBaseDeDadosComPowerQuery/Cadastro Lojas.xlsx
+++ b/003-importacaoETratamentoDeBaseDeDadosComPowerQuery/Cadastro Lojas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Power BI/Power BI Impressionador/Módulo Power Query (Novo)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jharbes\Documents\GitHub\hashtagPowerBI\003-importacaoETratamentoDeBaseDeDadosComPowerQuery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_FA66D272AA1066B08AF955C2714F872426B3E244" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7CBCFD2-8B82-4F63-B517-1055166E96D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3F10A2-9443-47B5-B220-546990E7E827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Loja</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>294681591</t>
+  </si>
+  <si>
+    <t>Rua Décio Vilares, 406 - Copacabana, Rio de Janeiro - RJ, 22045-050</t>
+  </si>
+  <si>
+    <t>Alon Pinheiro</t>
+  </si>
+  <si>
+    <t>28456321X</t>
   </si>
 </sst>
 </file>
@@ -209,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,11 +241,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +271,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,18 +556,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -558,7 +583,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -572,7 +597,7 @@
         <v>506215428</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -586,7 +611,7 @@
         <v>259267806</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -600,7 +625,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -614,7 +639,7 @@
         <v>259430602</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
@@ -628,7 +653,7 @@
         <v>198870966</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -642,7 +667,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -656,7 +681,7 @@
         <v>307641375</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -670,7 +695,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -684,7 +709,7 @@
         <v>247230364</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -698,7 +723,7 @@
         <v>328196186</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -712,7 +737,7 @@
         <v>369595269</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -726,7 +751,7 @@
         <v>335836902</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -738,6 +763,20 @@
       </c>
       <c r="D14" s="4">
         <v>486616964</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>